<commit_message>
Cambiando el problema 1b para leer datos desde Excel, quede en Lineas
</commit_message>
<xml_diff>
--- a/Tarea2/Case014.xlsx
+++ b/Tarea2/Case014.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barri\Documents\Operacion_Economica\Tarea2_Operacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Cursos\IEE3363 Aplicaciones\Tareas\Tarea 3\Solución\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12A5E6C-5FA5-46BA-8384-A05A76CF4008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="699" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="699"/>
   </bookViews>
   <sheets>
     <sheet name="Buses" sheetId="6" r:id="rId1"/>
@@ -22,25 +21,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Buses!$A$1:$E$16</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="91">
   <si>
     <t>Generator</t>
   </si>
@@ -310,12 +296,15 @@
   </si>
   <si>
     <t>Power Profile [MW]</t>
+  </si>
+  <si>
+    <t>Pmax for renewables is a reference of power availability</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -348,10 +337,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -374,7 +366,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -546,7 +538,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -718,7 +710,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1199,13 +1191,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1265,13 +1251,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1303,13 +1283,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1346,13 +1320,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1412,13 +1380,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1439,9 +1401,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1479,9 +1441,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1516,7 +1478,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1551,7 +1513,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1724,23 +1686,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1757,14 +1717,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>1.06</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>0.94</v>
       </c>
       <c r="D2">
@@ -1774,14 +1734,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>1.06</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>0.94</v>
       </c>
       <c r="D3">
@@ -1791,14 +1751,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>1.06</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>0.94</v>
       </c>
       <c r="D4">
@@ -1808,14 +1768,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>1.06</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>0.94</v>
       </c>
       <c r="D5">
@@ -1825,14 +1785,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>1.06</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>0.94</v>
       </c>
       <c r="D6">
@@ -1842,14 +1802,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>1.06</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>0.94</v>
       </c>
       <c r="D7">
@@ -1859,14 +1819,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>1.06</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>0.94</v>
       </c>
       <c r="D8">
@@ -1876,14 +1836,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>1.06</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>0.94</v>
       </c>
       <c r="D9">
@@ -1893,14 +1853,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>1.06</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>0.94</v>
       </c>
       <c r="D10">
@@ -1910,14 +1870,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>1.06</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>0.94</v>
       </c>
       <c r="D11">
@@ -1927,14 +1887,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>1.06</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>0.94</v>
       </c>
       <c r="D12">
@@ -1944,14 +1904,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>1.06</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>0.94</v>
       </c>
       <c r="D13">
@@ -1961,14 +1921,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>1.06</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="3">
         <v>0.94</v>
       </c>
       <c r="D14">
@@ -1978,14 +1938,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>1.06</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="3">
         <v>0.94</v>
       </c>
       <c r="D15">
@@ -1995,10 +1955,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2008,29 +1970,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AY19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="24" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="51" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="24" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="51" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -2038,7 +1998,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -2190,2135 +2150,2135 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2">
-        <v>0</v>
-      </c>
-      <c r="L3" s="2">
-        <v>0</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0</v>
-      </c>
-      <c r="N3" s="2">
-        <v>0</v>
-      </c>
-      <c r="O3" s="2">
-        <v>0</v>
-      </c>
-      <c r="P3" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>0</v>
-      </c>
-      <c r="R3" s="2">
-        <v>0</v>
-      </c>
-      <c r="S3" s="2">
-        <v>0</v>
-      </c>
-      <c r="T3" s="2">
-        <v>0</v>
-      </c>
-      <c r="U3" s="2">
-        <v>0</v>
-      </c>
-      <c r="V3" s="2">
-        <v>0</v>
-      </c>
-      <c r="W3" s="2">
-        <v>0</v>
-      </c>
-      <c r="X3" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="2">
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0</v>
+      </c>
+      <c r="O3" s="4">
+        <v>0</v>
+      </c>
+      <c r="P3" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>0</v>
+      </c>
+      <c r="R3" s="4">
+        <v>0</v>
+      </c>
+      <c r="S3" s="4">
+        <v>0</v>
+      </c>
+      <c r="T3" s="4">
+        <v>0</v>
+      </c>
+      <c r="U3" s="4">
+        <v>0</v>
+      </c>
+      <c r="V3" s="4">
+        <v>0</v>
+      </c>
+      <c r="W3" s="4">
+        <v>0</v>
+      </c>
+      <c r="X3" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="4">
         <v>0</v>
       </c>
       <c r="AA3" t="s">
         <v>19</v>
       </c>
-      <c r="AB3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AT3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AU3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AW3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AX3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AY3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.35">
+      <c r="AB3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="4">
         <v>21.7</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <v>17.695135135135139</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <v>15.550270270270273</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="4">
         <v>13.941621621621625</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="4">
         <v>13.405405405405409</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="4">
         <v>16.086486486486489</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="4">
         <v>18.767567567567571</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="4">
         <v>20.912432432432439</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="4">
         <v>21.984864864864868</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="4">
         <v>23.593513513513521</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="4">
         <v>23.861621621621627</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="4">
         <v>22.521081081081086</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="4">
         <v>21.448648648648653</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="4">
         <v>20.376216216216221</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="4">
         <v>23.593513513513521</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q4" s="4">
         <v>24.129729729729736</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4" s="4">
         <v>22.789189189189194</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4" s="4">
         <v>23.861621621621627</v>
       </c>
-      <c r="T4" s="2">
+      <c r="T4" s="4">
         <v>25.202162162162164</v>
       </c>
-      <c r="U4" s="2">
+      <c r="U4" s="4">
         <v>26.274594594594603</v>
       </c>
-      <c r="V4" s="2">
+      <c r="V4" s="4">
         <v>26.810810810810818</v>
       </c>
-      <c r="W4" s="2">
+      <c r="W4" s="4">
         <v>24.129729729729736</v>
       </c>
-      <c r="X4" s="2">
+      <c r="X4" s="4">
         <v>23.325405405405409</v>
       </c>
-      <c r="Y4" s="2">
+      <c r="Y4" s="4">
         <v>21.984864864864868</v>
       </c>
       <c r="AA4" t="s">
         <v>20</v>
       </c>
-      <c r="AB4" s="2">
+      <c r="AB4" s="4">
         <v>12.7</v>
       </c>
-      <c r="AC4" s="2">
+      <c r="AC4" s="4">
         <v>10.356138996138998</v>
       </c>
-      <c r="AD4" s="2">
+      <c r="AD4" s="4">
         <v>9.1008494208494231</v>
       </c>
-      <c r="AE4" s="2">
+      <c r="AE4" s="4">
         <v>8.1593822393822411</v>
       </c>
-      <c r="AF4" s="2">
+      <c r="AF4" s="4">
         <v>7.8455598455598468</v>
       </c>
-      <c r="AG4" s="2">
+      <c r="AG4" s="4">
         <v>9.4146718146718165</v>
       </c>
-      <c r="AH4" s="2">
+      <c r="AH4" s="4">
         <v>10.983783783783785</v>
       </c>
-      <c r="AI4" s="2">
+      <c r="AI4" s="4">
         <v>12.239073359073362</v>
       </c>
-      <c r="AJ4" s="2">
+      <c r="AJ4" s="4">
         <v>12.866718146718148</v>
       </c>
-      <c r="AK4" s="2">
+      <c r="AK4" s="4">
         <v>13.808185328185331</v>
       </c>
-      <c r="AL4" s="2">
+      <c r="AL4" s="4">
         <v>13.965096525096527</v>
       </c>
-      <c r="AM4" s="2">
+      <c r="AM4" s="4">
         <v>13.180540540540543</v>
       </c>
-      <c r="AN4" s="2">
+      <c r="AN4" s="4">
         <v>12.552895752895754</v>
       </c>
-      <c r="AO4" s="2">
+      <c r="AO4" s="4">
         <v>11.925250965250967</v>
       </c>
-      <c r="AP4" s="2">
+      <c r="AP4" s="4">
         <v>13.808185328185331</v>
       </c>
-      <c r="AQ4" s="2">
+      <c r="AQ4" s="4">
         <v>14.122007722007725</v>
       </c>
-      <c r="AR4" s="2">
+      <c r="AR4" s="4">
         <v>13.33745173745174</v>
       </c>
-      <c r="AS4" s="2">
+      <c r="AS4" s="4">
         <v>13.965096525096527</v>
       </c>
-      <c r="AT4" s="2">
+      <c r="AT4" s="4">
         <v>14.749652509652512</v>
       </c>
-      <c r="AU4" s="2">
+      <c r="AU4" s="4">
         <v>15.377297297297302</v>
       </c>
-      <c r="AV4" s="2">
+      <c r="AV4" s="4">
         <v>15.691119691119694</v>
       </c>
-      <c r="AW4" s="2">
+      <c r="AW4" s="4">
         <v>14.122007722007725</v>
       </c>
-      <c r="AX4" s="2">
+      <c r="AX4" s="4">
         <v>13.651274131274132</v>
       </c>
-      <c r="AY4" s="2">
+      <c r="AY4" s="4">
         <v>12.866718146718148</v>
       </c>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="4">
         <v>94.2</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="4">
         <v>76.814826254826272</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
         <v>67.503938223938235</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="4">
         <v>60.520772200772214</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="4">
         <v>58.193050193050205</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="4">
         <v>69.831660231660251</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="4">
         <v>81.470270270270291</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="4">
         <v>90.781158301158328</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="4">
         <v>95.436602316602333</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="4">
         <v>102.41976833976837</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="4">
         <v>103.58362934362937</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="4">
         <v>97.764324324324349</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="4">
         <v>93.10888030888033</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="4">
         <v>88.453436293436312</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="4">
         <v>102.41976833976837</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="Q5" s="4">
         <v>104.74749034749037</v>
       </c>
-      <c r="R5" s="2">
+      <c r="R5" s="4">
         <v>98.92818532818535</v>
       </c>
-      <c r="S5" s="2">
+      <c r="S5" s="4">
         <v>103.58362934362937</v>
       </c>
-      <c r="T5" s="2">
+      <c r="T5" s="4">
         <v>109.40293436293437</v>
       </c>
-      <c r="U5" s="2">
+      <c r="U5" s="4">
         <v>114.05837837837841</v>
       </c>
-      <c r="V5" s="2">
+      <c r="V5" s="4">
         <v>116.38610038610041</v>
       </c>
-      <c r="W5" s="2">
+      <c r="W5" s="4">
         <v>104.74749034749037</v>
       </c>
-      <c r="X5" s="2">
+      <c r="X5" s="4">
         <v>101.25590733590735</v>
       </c>
-      <c r="Y5" s="2">
+      <c r="Y5" s="4">
         <v>95.436602316602333</v>
       </c>
       <c r="AA5" t="s">
         <v>21</v>
       </c>
-      <c r="AB5" s="2">
+      <c r="AB5" s="4">
         <v>19</v>
       </c>
-      <c r="AC5" s="2">
+      <c r="AC5" s="4">
         <v>15.493436293436297</v>
       </c>
-      <c r="AD5" s="2">
+      <c r="AD5" s="4">
         <v>13.615444015444016</v>
       </c>
-      <c r="AE5" s="2">
+      <c r="AE5" s="4">
         <v>12.20694980694981</v>
       </c>
-      <c r="AF5" s="2">
+      <c r="AF5" s="4">
         <v>11.737451737451741</v>
       </c>
-      <c r="AG5" s="2">
+      <c r="AG5" s="4">
         <v>14.084942084942089</v>
       </c>
-      <c r="AH5" s="2">
+      <c r="AH5" s="4">
         <v>16.432432432432439</v>
       </c>
-      <c r="AI5" s="2">
+      <c r="AI5" s="4">
         <v>18.310424710424716</v>
       </c>
-      <c r="AJ5" s="2">
+      <c r="AJ5" s="4">
         <v>19.249420849420851</v>
       </c>
-      <c r="AK5" s="2">
+      <c r="AK5" s="4">
         <v>20.657915057915066</v>
       </c>
-      <c r="AL5" s="2">
+      <c r="AL5" s="4">
         <v>20.892664092664095</v>
       </c>
-      <c r="AM5" s="2">
+      <c r="AM5" s="4">
         <v>19.718918918918924</v>
       </c>
-      <c r="AN5" s="2">
+      <c r="AN5" s="4">
         <v>18.779922779922781</v>
       </c>
-      <c r="AO5" s="2">
+      <c r="AO5" s="4">
         <v>17.840926640926643</v>
       </c>
-      <c r="AP5" s="2">
+      <c r="AP5" s="4">
         <v>20.657915057915066</v>
       </c>
-      <c r="AQ5" s="2">
+      <c r="AQ5" s="4">
         <v>21.127413127413131</v>
       </c>
-      <c r="AR5" s="2">
+      <c r="AR5" s="4">
         <v>19.953667953667956</v>
       </c>
-      <c r="AS5" s="2">
+      <c r="AS5" s="4">
         <v>20.892664092664095</v>
       </c>
-      <c r="AT5" s="2">
+      <c r="AT5" s="4">
         <v>22.06640926640927</v>
       </c>
-      <c r="AU5" s="2">
+      <c r="AU5" s="4">
         <v>23.005405405405408</v>
       </c>
-      <c r="AV5" s="2">
+      <c r="AV5" s="4">
         <v>23.474903474903481</v>
       </c>
-      <c r="AW5" s="2">
+      <c r="AW5" s="4">
         <v>21.127413127413131</v>
       </c>
-      <c r="AX5" s="2">
+      <c r="AX5" s="4">
         <v>20.423166023166026</v>
       </c>
-      <c r="AY5" s="2">
+      <c r="AY5" s="4">
         <v>19.249420849420851</v>
       </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="4">
         <v>47.8</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="4">
         <v>38.978223938223948</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4">
         <v>34.253590733590741</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="4">
         <v>30.710115830115839</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="4">
         <v>29.528957528957534</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="4">
         <v>35.434749034749046</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="4">
         <v>41.340540540540552</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="4">
         <v>46.065173745173759</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="4">
         <v>48.427490347490355</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="4">
         <v>51.970965250965264</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="4">
         <v>52.561544401544417</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="4">
         <v>49.608648648648661</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="4">
         <v>47.246332046332057</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="4">
         <v>44.884015444015454</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="4">
         <v>51.970965250965264</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q6" s="4">
         <v>53.152123552123562</v>
       </c>
-      <c r="R6" s="2">
+      <c r="R6" s="4">
         <v>50.199227799227813</v>
       </c>
-      <c r="S6" s="2">
+      <c r="S6" s="4">
         <v>52.561544401544417</v>
       </c>
-      <c r="T6" s="2">
+      <c r="T6" s="4">
         <v>55.514440154440159</v>
       </c>
-      <c r="U6" s="2">
+      <c r="U6" s="4">
         <v>57.876756756756777</v>
       </c>
-      <c r="V6" s="2">
+      <c r="V6" s="4">
         <v>59.057915057915068</v>
       </c>
-      <c r="W6" s="2">
+      <c r="W6" s="4">
         <v>53.152123552123562</v>
       </c>
-      <c r="X6" s="2">
+      <c r="X6" s="4">
         <v>51.380386100386104</v>
       </c>
-      <c r="Y6" s="2">
+      <c r="Y6" s="4">
         <v>48.427490347490355</v>
       </c>
       <c r="AA6" t="s">
         <v>22</v>
       </c>
-      <c r="AB6" s="2">
+      <c r="AB6" s="4">
         <v>-3.9</v>
       </c>
-      <c r="AC6" s="2">
+      <c r="AC6" s="4">
         <v>-3.1802316602316614</v>
       </c>
-      <c r="AD6" s="2">
+      <c r="AD6" s="4">
         <v>-2.7947490347490351</v>
       </c>
-      <c r="AE6" s="2">
+      <c r="AE6" s="4">
         <v>-2.5056370656370666</v>
       </c>
-      <c r="AF6" s="2">
+      <c r="AF6" s="4">
         <v>-2.4092664092664098</v>
       </c>
-      <c r="AG6" s="2">
+      <c r="AG6" s="4">
         <v>-2.8911196911196924</v>
       </c>
-      <c r="AH6" s="2">
+      <c r="AH6" s="4">
         <v>-3.372972972972974</v>
       </c>
-      <c r="AI6" s="2">
+      <c r="AI6" s="4">
         <v>-3.7584555984555998</v>
       </c>
-      <c r="AJ6" s="2">
+      <c r="AJ6" s="4">
         <v>-3.9511969111969121</v>
       </c>
-      <c r="AK6" s="2">
+      <c r="AK6" s="4">
         <v>-4.2403088803088815</v>
       </c>
-      <c r="AL6" s="2">
+      <c r="AL6" s="4">
         <v>-4.2884942084942104</v>
       </c>
-      <c r="AM6" s="2">
+      <c r="AM6" s="4">
         <v>-4.0475675675675689</v>
       </c>
-      <c r="AN6" s="2">
+      <c r="AN6" s="4">
         <v>-3.8548262548262557</v>
       </c>
-      <c r="AO6" s="2">
+      <c r="AO6" s="4">
         <v>-3.6620849420849431</v>
       </c>
-      <c r="AP6" s="2">
+      <c r="AP6" s="4">
         <v>-4.2403088803088815</v>
       </c>
-      <c r="AQ6" s="2">
+      <c r="AQ6" s="4">
         <v>-4.3366795366795374</v>
       </c>
-      <c r="AR6" s="2">
+      <c r="AR6" s="4">
         <v>-4.0957528957528968</v>
       </c>
-      <c r="AS6" s="2">
+      <c r="AS6" s="4">
         <v>-4.2884942084942104</v>
       </c>
-      <c r="AT6" s="2">
+      <c r="AT6" s="4">
         <v>-4.5294208494208501</v>
       </c>
-      <c r="AU6" s="2">
+      <c r="AU6" s="4">
         <v>-4.7221621621621646</v>
       </c>
-      <c r="AV6" s="2">
+      <c r="AV6" s="4">
         <v>-4.8185328185328196</v>
       </c>
-      <c r="AW6" s="2">
+      <c r="AW6" s="4">
         <v>-4.3366795366795374</v>
       </c>
-      <c r="AX6" s="2">
+      <c r="AX6" s="4">
         <v>-4.1921235521235527</v>
       </c>
-      <c r="AY6" s="2">
+      <c r="AY6" s="4">
         <v>-3.9511969111969121</v>
       </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="4">
         <v>7.6</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="4">
         <v>6.1973745173745192</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
         <v>5.4461776061776073</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="4">
         <v>4.8827799227799238</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="4">
         <v>4.6949806949806963</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="4">
         <v>5.6339768339768348</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="4">
         <v>6.5729729729729742</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="4">
         <v>7.3241698841698861</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="4">
         <v>7.6997683397683412</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="4">
         <v>8.2631660231660256</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="4">
         <v>8.3570656370656398</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="4">
         <v>7.8875675675675696</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="4">
         <v>7.5119691119691137</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="4">
         <v>7.1363706563706577</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="4">
         <v>8.2631660231660256</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="Q7" s="4">
         <v>8.4509652509652522</v>
       </c>
-      <c r="R7" s="2">
+      <c r="R7" s="4">
         <v>7.9814671814671829</v>
       </c>
-      <c r="S7" s="2">
+      <c r="S7" s="4">
         <v>8.3570656370656398</v>
       </c>
-      <c r="T7" s="2">
+      <c r="T7" s="4">
         <v>8.8265637065637073</v>
       </c>
-      <c r="U7" s="2">
+      <c r="U7" s="4">
         <v>9.2021621621621641</v>
       </c>
-      <c r="V7" s="2">
+      <c r="V7" s="4">
         <v>9.3899613899613925</v>
       </c>
-      <c r="W7" s="2">
+      <c r="W7" s="4">
         <v>8.4509652509652522</v>
       </c>
-      <c r="X7" s="2">
+      <c r="X7" s="4">
         <v>8.1692664092664096</v>
       </c>
-      <c r="Y7" s="2">
+      <c r="Y7" s="4">
         <v>7.6997683397683412</v>
       </c>
       <c r="AA7" t="s">
         <v>23</v>
       </c>
-      <c r="AB7" s="2">
+      <c r="AB7" s="4">
         <v>1.6</v>
       </c>
-      <c r="AC7" s="2">
+      <c r="AC7" s="4">
         <v>1.3047104247104253</v>
       </c>
-      <c r="AD7" s="2">
+      <c r="AD7" s="4">
         <v>1.1465637065637071</v>
       </c>
-      <c r="AE7" s="2">
+      <c r="AE7" s="4">
         <v>1.0279536679536683</v>
       </c>
-      <c r="AF7" s="2">
+      <c r="AF7" s="4">
         <v>0.98841698841698877</v>
       </c>
-      <c r="AG7" s="2">
+      <c r="AG7" s="4">
         <v>1.1861003861003863</v>
       </c>
-      <c r="AH7" s="2">
+      <c r="AH7" s="4">
         <v>1.3837837837837843</v>
       </c>
-      <c r="AI7" s="2">
+      <c r="AI7" s="4">
         <v>1.5419305019305025</v>
       </c>
-      <c r="AJ7" s="2">
+      <c r="AJ7" s="4">
         <v>1.6210038610038615</v>
       </c>
-      <c r="AK7" s="2">
+      <c r="AK7" s="4">
         <v>1.7396138996139003</v>
       </c>
-      <c r="AL7" s="2">
+      <c r="AL7" s="4">
         <v>1.7593822393822403</v>
       </c>
-      <c r="AM7" s="2">
+      <c r="AM7" s="4">
         <v>1.6605405405405413</v>
       </c>
-      <c r="AN7" s="2">
+      <c r="AN7" s="4">
         <v>1.5814671814671821</v>
       </c>
-      <c r="AO7" s="2">
+      <c r="AO7" s="4">
         <v>1.5023938223938229</v>
       </c>
-      <c r="AP7" s="2">
+      <c r="AP7" s="4">
         <v>1.7396138996139003</v>
       </c>
-      <c r="AQ7" s="2">
+      <c r="AQ7" s="4">
         <v>1.7791505791505795</v>
       </c>
-      <c r="AR7" s="2">
+      <c r="AR7" s="4">
         <v>1.6803088803088808</v>
       </c>
-      <c r="AS7" s="2">
+      <c r="AS7" s="4">
         <v>1.7593822393822403</v>
       </c>
-      <c r="AT7" s="2">
+      <c r="AT7" s="4">
         <v>1.8582239382239387</v>
       </c>
-      <c r="AU7" s="2">
+      <c r="AU7" s="4">
         <v>1.9372972972972977</v>
       </c>
-      <c r="AV7" s="2">
+      <c r="AV7" s="4">
         <v>1.9768339768339775</v>
       </c>
-      <c r="AW7" s="2">
+      <c r="AW7" s="4">
         <v>1.7791505791505795</v>
       </c>
-      <c r="AX7" s="2">
+      <c r="AX7" s="4">
         <v>1.7198455598455602</v>
       </c>
-      <c r="AY7" s="2">
+      <c r="AY7" s="4">
         <v>1.6210038610038615</v>
       </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="4">
         <v>11.2</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="4">
         <v>9.1329729729729756</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="4">
         <v>8.0259459459459475</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="4">
         <v>7.1956756756756777</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="4">
         <v>6.9189189189189202</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="4">
         <v>8.3027027027027049</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="4">
         <v>9.6864864864864888</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="4">
         <v>10.793513513513517</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="4">
         <v>11.347027027027028</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="4">
         <v>12.177297297297301</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="4">
         <v>12.31567567567568</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="4">
         <v>11.623783783783788</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="4">
         <v>11.070270270270273</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O8" s="4">
         <v>10.516756756756758</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="4">
         <v>12.177297297297301</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="Q8" s="4">
         <v>12.454054054054057</v>
       </c>
-      <c r="R8" s="2">
+      <c r="R8" s="4">
         <v>11.762162162162165</v>
       </c>
-      <c r="S8" s="2">
+      <c r="S8" s="4">
         <v>12.31567567567568</v>
       </c>
-      <c r="T8" s="2">
+      <c r="T8" s="4">
         <v>13.007567567567568</v>
       </c>
-      <c r="U8" s="2">
+      <c r="U8" s="4">
         <v>13.561081081081085</v>
       </c>
-      <c r="V8" s="2">
+      <c r="V8" s="4">
         <v>13.83783783783784</v>
       </c>
-      <c r="W8" s="2">
+      <c r="W8" s="4">
         <v>12.454054054054057</v>
       </c>
-      <c r="X8" s="2">
+      <c r="X8" s="4">
         <v>12.03891891891892</v>
       </c>
-      <c r="Y8" s="2">
+      <c r="Y8" s="4">
         <v>11.347027027027028</v>
       </c>
       <c r="AA8" t="s">
         <v>24</v>
       </c>
-      <c r="AB8" s="2">
+      <c r="AB8" s="4">
         <v>7.5000000000000009</v>
       </c>
-      <c r="AC8" s="2">
+      <c r="AC8" s="4">
         <v>6.1158301158301187</v>
       </c>
-      <c r="AD8" s="2">
+      <c r="AD8" s="4">
         <v>5.3745173745173762</v>
       </c>
-      <c r="AE8" s="2">
+      <c r="AE8" s="4">
         <v>4.8185328185328204</v>
       </c>
-      <c r="AF8" s="2">
+      <c r="AF8" s="4">
         <v>4.6332046332046346</v>
       </c>
-      <c r="AG8" s="2">
+      <c r="AG8" s="4">
         <v>5.5598455598455621</v>
       </c>
-      <c r="AH8" s="2">
+      <c r="AH8" s="4">
         <v>6.4864864864864877</v>
       </c>
-      <c r="AI8" s="2">
+      <c r="AI8" s="4">
         <v>7.2277992277992302</v>
       </c>
-      <c r="AJ8" s="2">
+      <c r="AJ8" s="4">
         <v>7.5984555984556001</v>
       </c>
-      <c r="AK8" s="2">
+      <c r="AK8" s="4">
         <v>8.1544401544401577</v>
       </c>
-      <c r="AL8" s="2">
+      <c r="AL8" s="4">
         <v>8.2471042471042502</v>
       </c>
-      <c r="AM8" s="2">
+      <c r="AM8" s="4">
         <v>7.7837837837837869</v>
       </c>
-      <c r="AN8" s="2">
+      <c r="AN8" s="4">
         <v>7.4131274131274152</v>
       </c>
-      <c r="AO8" s="2">
+      <c r="AO8" s="4">
         <v>7.0424710424710435</v>
       </c>
-      <c r="AP8" s="2">
+      <c r="AP8" s="4">
         <v>8.1544401544401577</v>
       </c>
-      <c r="AQ8" s="2">
+      <c r="AQ8" s="4">
         <v>8.3397683397683409</v>
       </c>
-      <c r="AR8" s="2">
+      <c r="AR8" s="4">
         <v>7.8764478764478794</v>
       </c>
-      <c r="AS8" s="2">
+      <c r="AS8" s="4">
         <v>8.2471042471042502</v>
       </c>
-      <c r="AT8" s="2">
+      <c r="AT8" s="4">
         <v>8.7104247104247108</v>
       </c>
-      <c r="AU8" s="2">
+      <c r="AU8" s="4">
         <v>9.0810810810810842</v>
       </c>
-      <c r="AV8" s="2">
+      <c r="AV8" s="4">
         <v>9.2664092664092692</v>
       </c>
-      <c r="AW8" s="2">
+      <c r="AW8" s="4">
         <v>8.3397683397683409</v>
       </c>
-      <c r="AX8" s="2">
+      <c r="AX8" s="4">
         <v>8.0617760617760634</v>
       </c>
-      <c r="AY8" s="2">
+      <c r="AY8" s="4">
         <v>7.5984555984556001</v>
       </c>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0</v>
-      </c>
-      <c r="J9" s="2">
-        <v>0</v>
-      </c>
-      <c r="K9" s="2">
-        <v>0</v>
-      </c>
-      <c r="L9" s="2">
-        <v>0</v>
-      </c>
-      <c r="M9" s="2">
-        <v>0</v>
-      </c>
-      <c r="N9" s="2">
-        <v>0</v>
-      </c>
-      <c r="O9" s="2">
-        <v>0</v>
-      </c>
-      <c r="P9" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>0</v>
-      </c>
-      <c r="R9" s="2">
-        <v>0</v>
-      </c>
-      <c r="S9" s="2">
-        <v>0</v>
-      </c>
-      <c r="T9" s="2">
-        <v>0</v>
-      </c>
-      <c r="U9" s="2">
-        <v>0</v>
-      </c>
-      <c r="V9" s="2">
-        <v>0</v>
-      </c>
-      <c r="W9" s="2">
-        <v>0</v>
-      </c>
-      <c r="X9" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="2">
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0</v>
+      </c>
+      <c r="N9" s="4">
+        <v>0</v>
+      </c>
+      <c r="O9" s="4">
+        <v>0</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>0</v>
+      </c>
+      <c r="R9" s="4">
+        <v>0</v>
+      </c>
+      <c r="S9" s="4">
+        <v>0</v>
+      </c>
+      <c r="T9" s="4">
+        <v>0</v>
+      </c>
+      <c r="U9" s="4">
+        <v>0</v>
+      </c>
+      <c r="V9" s="4">
+        <v>0</v>
+      </c>
+      <c r="W9" s="4">
+        <v>0</v>
+      </c>
+      <c r="X9" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="4">
         <v>0</v>
       </c>
       <c r="AA9" t="s">
         <v>25</v>
       </c>
-      <c r="AB9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AI9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AN9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AP9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AQ9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AR9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AS9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AT9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AU9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AW9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AX9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AY9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.35">
+      <c r="AB9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2">
-        <v>0</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0</v>
-      </c>
-      <c r="K10" s="2">
-        <v>0</v>
-      </c>
-      <c r="L10" s="2">
-        <v>0</v>
-      </c>
-      <c r="M10" s="2">
-        <v>0</v>
-      </c>
-      <c r="N10" s="2">
-        <v>0</v>
-      </c>
-      <c r="O10" s="2">
-        <v>0</v>
-      </c>
-      <c r="P10" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>0</v>
-      </c>
-      <c r="R10" s="2">
-        <v>0</v>
-      </c>
-      <c r="S10" s="2">
-        <v>0</v>
-      </c>
-      <c r="T10" s="2">
-        <v>0</v>
-      </c>
-      <c r="U10" s="2">
-        <v>0</v>
-      </c>
-      <c r="V10" s="2">
-        <v>0</v>
-      </c>
-      <c r="W10" s="2">
-        <v>0</v>
-      </c>
-      <c r="X10" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="2">
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+      <c r="M10" s="4">
+        <v>0</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0</v>
+      </c>
+      <c r="O10" s="4">
+        <v>0</v>
+      </c>
+      <c r="P10" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>0</v>
+      </c>
+      <c r="R10" s="4">
+        <v>0</v>
+      </c>
+      <c r="S10" s="4">
+        <v>0</v>
+      </c>
+      <c r="T10" s="4">
+        <v>0</v>
+      </c>
+      <c r="U10" s="4">
+        <v>0</v>
+      </c>
+      <c r="V10" s="4">
+        <v>0</v>
+      </c>
+      <c r="W10" s="4">
+        <v>0</v>
+      </c>
+      <c r="X10" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="4">
         <v>0</v>
       </c>
       <c r="AA10" t="s">
         <v>26</v>
       </c>
-      <c r="AB10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AI10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AN10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AP10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AQ10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AR10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AS10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AT10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AU10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AW10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AX10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AY10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.35">
+      <c r="AB10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="4">
         <v>29.5</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="4">
         <v>24.055598455598464</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="4">
         <v>21.139768339768342</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="4">
         <v>18.952895752895756</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="4">
         <v>18.223938223938227</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="4">
         <v>21.868725868725875</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="4">
         <v>25.513513513513519</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="4">
         <v>28.429343629343638</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="4">
         <v>29.88725868725869</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="4">
         <v>32.074131274131283</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="4">
         <v>32.438610038610044</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11" s="4">
         <v>30.616216216216223</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N11" s="4">
         <v>29.158301158301164</v>
       </c>
-      <c r="O11" s="2">
+      <c r="O11" s="4">
         <v>27.700386100386105</v>
       </c>
-      <c r="P11" s="2">
+      <c r="P11" s="4">
         <v>32.074131274131283</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="Q11" s="4">
         <v>32.803088803088812</v>
       </c>
-      <c r="R11" s="2">
+      <c r="R11" s="4">
         <v>30.980694980694988</v>
       </c>
-      <c r="S11" s="2">
+      <c r="S11" s="4">
         <v>32.438610038610044</v>
       </c>
-      <c r="T11" s="2">
+      <c r="T11" s="4">
         <v>34.261003861003864</v>
       </c>
-      <c r="U11" s="2">
+      <c r="U11" s="4">
         <v>35.718918918918931</v>
       </c>
-      <c r="V11" s="2">
+      <c r="V11" s="4">
         <v>36.447876447876453</v>
       </c>
-      <c r="W11" s="2">
+      <c r="W11" s="4">
         <v>32.803088803088812</v>
       </c>
-      <c r="X11" s="2">
+      <c r="X11" s="4">
         <v>31.709652509652514</v>
       </c>
-      <c r="Y11" s="2">
+      <c r="Y11" s="4">
         <v>29.88725868725869</v>
       </c>
       <c r="AA11" t="s">
         <v>27</v>
       </c>
-      <c r="AB11" s="2">
+      <c r="AB11" s="4">
         <v>16.600000000000001</v>
       </c>
-      <c r="AC11" s="2">
+      <c r="AC11" s="4">
         <v>13.536370656370663</v>
       </c>
-      <c r="AD11" s="2">
+      <c r="AD11" s="4">
         <v>11.895598455598456</v>
       </c>
-      <c r="AE11" s="2">
+      <c r="AE11" s="4">
         <v>10.665019305019309</v>
       </c>
-      <c r="AF11" s="2">
+      <c r="AF11" s="4">
         <v>10.254826254826257</v>
       </c>
-      <c r="AG11" s="2">
+      <c r="AG11" s="4">
         <v>12.305791505791511</v>
       </c>
-      <c r="AH11" s="2">
+      <c r="AH11" s="4">
         <v>14.356756756756763</v>
       </c>
-      <c r="AI11" s="2">
+      <c r="AI11" s="4">
         <v>15.997528957528964</v>
       </c>
-      <c r="AJ11" s="2">
+      <c r="AJ11" s="4">
         <v>16.817915057915062</v>
       </c>
-      <c r="AK11" s="2">
+      <c r="AK11" s="4">
         <v>18.048494208494215</v>
       </c>
-      <c r="AL11" s="2">
+      <c r="AL11" s="4">
         <v>18.253590733590737</v>
       </c>
-      <c r="AM11" s="2">
+      <c r="AM11" s="4">
         <v>17.228108108108113</v>
       </c>
-      <c r="AN11" s="2">
+      <c r="AN11" s="4">
         <v>16.407722007722015</v>
       </c>
-      <c r="AO11" s="2">
+      <c r="AO11" s="4">
         <v>15.587335907335911</v>
       </c>
-      <c r="AP11" s="2">
+      <c r="AP11" s="4">
         <v>18.048494208494215</v>
       </c>
-      <c r="AQ11" s="2">
+      <c r="AQ11" s="4">
         <v>18.458687258687267</v>
       </c>
-      <c r="AR11" s="2">
+      <c r="AR11" s="4">
         <v>17.433204633204639</v>
       </c>
-      <c r="AS11" s="2">
+      <c r="AS11" s="4">
         <v>18.253590733590737</v>
       </c>
-      <c r="AT11" s="2">
+      <c r="AT11" s="4">
         <v>19.279073359073362</v>
       </c>
-      <c r="AU11" s="2">
+      <c r="AU11" s="4">
         <v>20.099459459459467</v>
       </c>
-      <c r="AV11" s="2">
+      <c r="AV11" s="4">
         <v>20.509652509652515</v>
       </c>
-      <c r="AW11" s="2">
+      <c r="AW11" s="4">
         <v>18.458687258687267</v>
       </c>
-      <c r="AX11" s="2">
+      <c r="AX11" s="4">
         <v>17.843397683397686</v>
       </c>
-      <c r="AY11" s="2">
+      <c r="AY11" s="4">
         <v>16.817915057915062</v>
       </c>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="4">
         <v>9</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="4">
         <v>7.3389961389961407</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="4">
         <v>6.4494208494208509</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="4">
         <v>5.7822393822393838</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="4">
         <v>5.5598455598455612</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="4">
         <v>6.6718146718146727</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="4">
         <v>7.7837837837837851</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="4">
         <v>8.6733590733590766</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="4">
         <v>9.1181467181467184</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="4">
         <v>9.7853281853281882</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="4">
         <v>9.8965250965250995</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="4">
         <v>9.3405405405405428</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="4">
         <v>8.8957528957528975</v>
       </c>
-      <c r="O12" s="2">
+      <c r="O12" s="4">
         <v>8.4509652509652522</v>
       </c>
-      <c r="P12" s="2">
+      <c r="P12" s="4">
         <v>9.7853281853281882</v>
       </c>
-      <c r="Q12" s="2">
+      <c r="Q12" s="4">
         <v>10.007722007722009</v>
       </c>
-      <c r="R12" s="2">
+      <c r="R12" s="4">
         <v>9.4517374517374542</v>
       </c>
-      <c r="S12" s="2">
+      <c r="S12" s="4">
         <v>9.8965250965250995</v>
       </c>
-      <c r="T12" s="2">
+      <c r="T12" s="4">
         <v>10.452509652509653</v>
       </c>
-      <c r="U12" s="2">
+      <c r="U12" s="4">
         <v>10.8972972972973</v>
       </c>
-      <c r="V12" s="2">
+      <c r="V12" s="4">
         <v>11.119691119691122</v>
       </c>
-      <c r="W12" s="2">
+      <c r="W12" s="4">
         <v>10.007722007722009</v>
       </c>
-      <c r="X12" s="2">
+      <c r="X12" s="4">
         <v>9.674131274131275</v>
       </c>
-      <c r="Y12" s="2">
+      <c r="Y12" s="4">
         <v>9.1181467181467184</v>
       </c>
       <c r="AA12" t="s">
         <v>28</v>
       </c>
-      <c r="AB12" s="2">
+      <c r="AB12" s="4">
         <v>5.8</v>
       </c>
-      <c r="AC12" s="2">
+      <c r="AC12" s="4">
         <v>4.7295752895752905</v>
       </c>
-      <c r="AD12" s="2">
+      <c r="AD12" s="4">
         <v>4.1562934362934367</v>
       </c>
-      <c r="AE12" s="2">
+      <c r="AE12" s="4">
         <v>3.7263320463320477</v>
       </c>
-      <c r="AF12" s="2">
+      <c r="AF12" s="4">
         <v>3.5830115830115838</v>
       </c>
-      <c r="AG12" s="2">
+      <c r="AG12" s="4">
         <v>4.2996138996138997</v>
       </c>
-      <c r="AH12" s="2">
+      <c r="AH12" s="4">
         <v>5.0162162162162174</v>
       </c>
-      <c r="AI12" s="2">
+      <c r="AI12" s="4">
         <v>5.5894980694980712</v>
       </c>
-      <c r="AJ12" s="2">
+      <c r="AJ12" s="4">
         <v>5.8761389961389963</v>
       </c>
-      <c r="AK12" s="2">
+      <c r="AK12" s="4">
         <v>6.3061003861003879</v>
       </c>
-      <c r="AL12" s="2">
+      <c r="AL12" s="4">
         <v>6.377760617760619</v>
       </c>
-      <c r="AM12" s="2">
+      <c r="AM12" s="4">
         <v>6.019459459459461</v>
       </c>
-      <c r="AN12" s="2">
+      <c r="AN12" s="4">
         <v>5.7328185328185342</v>
       </c>
-      <c r="AO12" s="2">
+      <c r="AO12" s="4">
         <v>5.4461776061776073</v>
       </c>
-      <c r="AP12" s="2">
+      <c r="AP12" s="4">
         <v>6.3061003861003879</v>
       </c>
-      <c r="AQ12" s="2">
+      <c r="AQ12" s="4">
         <v>6.44942084942085</v>
       </c>
-      <c r="AR12" s="2">
+      <c r="AR12" s="4">
         <v>6.0911196911196921</v>
       </c>
-      <c r="AS12" s="2">
+      <c r="AS12" s="4">
         <v>6.377760617760619</v>
       </c>
-      <c r="AT12" s="2">
+      <c r="AT12" s="4">
         <v>6.736061776061776</v>
       </c>
-      <c r="AU12" s="2">
+      <c r="AU12" s="4">
         <v>7.0227027027027047</v>
       </c>
-      <c r="AV12" s="2">
+      <c r="AV12" s="4">
         <v>7.1660231660231677</v>
       </c>
-      <c r="AW12" s="2">
+      <c r="AW12" s="4">
         <v>6.44942084942085</v>
       </c>
-      <c r="AX12" s="2">
+      <c r="AX12" s="4">
         <v>6.2344401544401542</v>
       </c>
-      <c r="AY12" s="2">
+      <c r="AY12" s="4">
         <v>5.8761389961389963</v>
       </c>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="4">
         <v>3.5</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="4">
         <v>2.8540540540540547</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="4">
         <v>2.5081081081081087</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="4">
         <v>2.2486486486486492</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="4">
         <v>2.1621621621621627</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="4">
         <v>2.5945945945945952</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="4">
         <v>3.0270270270270276</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="4">
         <v>3.372972972972974</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="4">
         <v>3.5459459459459461</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="4">
         <v>3.8054054054054065</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13" s="4">
         <v>3.8486486486486493</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M13" s="4">
         <v>3.6324324324324331</v>
       </c>
-      <c r="N13" s="2">
+      <c r="N13" s="4">
         <v>3.4594594594594601</v>
       </c>
-      <c r="O13" s="2">
+      <c r="O13" s="4">
         <v>3.2864864864864871</v>
       </c>
-      <c r="P13" s="2">
+      <c r="P13" s="4">
         <v>3.8054054054054065</v>
       </c>
-      <c r="Q13" s="2">
+      <c r="Q13" s="4">
         <v>3.8918918918918926</v>
       </c>
-      <c r="R13" s="2">
+      <c r="R13" s="4">
         <v>3.6756756756756763</v>
       </c>
-      <c r="S13" s="2">
+      <c r="S13" s="4">
         <v>3.8486486486486493</v>
       </c>
-      <c r="T13" s="2">
+      <c r="T13" s="4">
         <v>4.0648648648648651</v>
       </c>
-      <c r="U13" s="2">
+      <c r="U13" s="4">
         <v>4.237837837837839</v>
       </c>
-      <c r="V13" s="2">
+      <c r="V13" s="4">
         <v>4.3243243243243255</v>
       </c>
-      <c r="W13" s="2">
+      <c r="W13" s="4">
         <v>3.8918918918918926</v>
       </c>
-      <c r="X13" s="2">
+      <c r="X13" s="4">
         <v>3.7621621621621624</v>
       </c>
-      <c r="Y13" s="2">
+      <c r="Y13" s="4">
         <v>3.5459459459459461</v>
       </c>
       <c r="AA13" t="s">
         <v>29</v>
       </c>
-      <c r="AB13" s="2">
+      <c r="AB13" s="4">
         <v>1.8</v>
       </c>
-      <c r="AC13" s="2">
+      <c r="AC13" s="4">
         <v>1.467799227799228</v>
       </c>
-      <c r="AD13" s="2">
+      <c r="AD13" s="4">
         <v>1.2898841698841701</v>
       </c>
-      <c r="AE13" s="2">
+      <c r="AE13" s="4">
         <v>1.1564478764478767</v>
       </c>
-      <c r="AF13" s="2">
+      <c r="AF13" s="4">
         <v>1.1119691119691122</v>
       </c>
-      <c r="AG13" s="2">
+      <c r="AG13" s="4">
         <v>1.3343629343629346</v>
       </c>
-      <c r="AH13" s="2">
+      <c r="AH13" s="4">
         <v>1.5567567567567571</v>
       </c>
-      <c r="AI13" s="2">
+      <c r="AI13" s="4">
         <v>1.7346718146718152</v>
       </c>
-      <c r="AJ13" s="2">
+      <c r="AJ13" s="4">
         <v>1.8236293436293438</v>
       </c>
-      <c r="AK13" s="2">
+      <c r="AK13" s="4">
         <v>1.9570656370656376</v>
       </c>
-      <c r="AL13" s="2">
+      <c r="AL13" s="4">
         <v>1.9793050193050197</v>
       </c>
-      <c r="AM13" s="2">
+      <c r="AM13" s="4">
         <v>1.8681081081081086</v>
       </c>
-      <c r="AN13" s="2">
+      <c r="AN13" s="4">
         <v>1.7791505791505795</v>
       </c>
-      <c r="AO13" s="2">
+      <c r="AO13" s="4">
         <v>1.6901930501930504</v>
       </c>
-      <c r="AP13" s="2">
+      <c r="AP13" s="4">
         <v>1.9570656370656376</v>
       </c>
-      <c r="AQ13" s="2">
+      <c r="AQ13" s="4">
         <v>2.0015444015444017</v>
       </c>
-      <c r="AR13" s="2">
+      <c r="AR13" s="4">
         <v>1.8903474903474908</v>
       </c>
-      <c r="AS13" s="2">
+      <c r="AS13" s="4">
         <v>1.9793050193050197</v>
       </c>
-      <c r="AT13" s="2">
+      <c r="AT13" s="4">
         <v>2.0905019305019308</v>
       </c>
-      <c r="AU13" s="2">
+      <c r="AU13" s="4">
         <v>2.1794594594594598</v>
       </c>
-      <c r="AV13" s="2">
+      <c r="AV13" s="4">
         <v>2.2239382239382244</v>
       </c>
-      <c r="AW13" s="2">
+      <c r="AW13" s="4">
         <v>2.0015444015444017</v>
       </c>
-      <c r="AX13" s="2">
+      <c r="AX13" s="4">
         <v>1.9348262548262549</v>
       </c>
-      <c r="AY13" s="2">
+      <c r="AY13" s="4">
         <v>1.8236293436293438</v>
       </c>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="4">
         <v>6.1</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="4">
         <v>4.9742084942084954</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="4">
         <v>4.3712741312741317</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="4">
         <v>3.91907335907336</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="4">
         <v>3.7683397683397688</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="4">
         <v>4.5220077220077233</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="4">
         <v>5.2756756756756769</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="4">
         <v>5.8786100386100406</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="4">
         <v>6.1800772200772203</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="4">
         <v>6.6322779922779942</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="4">
         <v>6.7076447876447896</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="4">
         <v>6.3308108108108119</v>
       </c>
-      <c r="N14" s="2">
+      <c r="N14" s="4">
         <v>6.0293436293436304</v>
       </c>
-      <c r="O14" s="2">
+      <c r="O14" s="4">
         <v>5.727876447876449</v>
       </c>
-      <c r="P14" s="2">
+      <c r="P14" s="4">
         <v>6.6322779922779942</v>
       </c>
-      <c r="Q14" s="2">
+      <c r="Q14" s="4">
         <v>6.783011583011584</v>
       </c>
-      <c r="R14" s="2">
+      <c r="R14" s="4">
         <v>6.4061776061776072</v>
       </c>
-      <c r="S14" s="2">
+      <c r="S14" s="4">
         <v>6.7076447876447896</v>
       </c>
-      <c r="T14" s="2">
+      <c r="T14" s="4">
         <v>7.0844787644787646</v>
       </c>
-      <c r="U14" s="2">
+      <c r="U14" s="4">
         <v>7.3859459459459478</v>
       </c>
-      <c r="V14" s="2">
+      <c r="V14" s="4">
         <v>7.5366795366795376</v>
       </c>
-      <c r="W14" s="2">
+      <c r="W14" s="4">
         <v>6.783011583011584</v>
       </c>
-      <c r="X14" s="2">
+      <c r="X14" s="4">
         <v>6.5569111969111979</v>
       </c>
-      <c r="Y14" s="2">
+      <c r="Y14" s="4">
         <v>6.1800772200772203</v>
       </c>
       <c r="AA14" t="s">
         <v>30</v>
       </c>
-      <c r="AB14" s="2">
+      <c r="AB14" s="4">
         <v>1.6</v>
       </c>
-      <c r="AC14" s="2">
+      <c r="AC14" s="4">
         <v>1.3047104247104251</v>
       </c>
-      <c r="AD14" s="2">
+      <c r="AD14" s="4">
         <v>1.1465637065637069</v>
       </c>
-      <c r="AE14" s="2">
+      <c r="AE14" s="4">
         <v>1.0279536679536683</v>
       </c>
-      <c r="AF14" s="2">
+      <c r="AF14" s="4">
         <v>0.98841698841698866</v>
       </c>
-      <c r="AG14" s="2">
+      <c r="AG14" s="4">
         <v>1.1861003861003867</v>
       </c>
-      <c r="AH14" s="2">
+      <c r="AH14" s="4">
         <v>1.3837837837837843</v>
       </c>
-      <c r="AI14" s="2">
+      <c r="AI14" s="4">
         <v>1.5419305019305025</v>
       </c>
-      <c r="AJ14" s="2">
+      <c r="AJ14" s="4">
         <v>1.6210038610038611</v>
       </c>
-      <c r="AK14" s="2">
+      <c r="AK14" s="4">
         <v>1.7396138996139006</v>
       </c>
-      <c r="AL14" s="2">
+      <c r="AL14" s="4">
         <v>1.75938223938224</v>
       </c>
-      <c r="AM14" s="2">
+      <c r="AM14" s="4">
         <v>1.6605405405405409</v>
       </c>
-      <c r="AN14" s="2">
+      <c r="AN14" s="4">
         <v>1.5814671814671819</v>
       </c>
-      <c r="AO14" s="2">
+      <c r="AO14" s="4">
         <v>1.5023938223938227</v>
       </c>
-      <c r="AP14" s="2">
+      <c r="AP14" s="4">
         <v>1.7396138996139006</v>
       </c>
-      <c r="AQ14" s="2">
+      <c r="AQ14" s="4">
         <v>1.7791505791505797</v>
       </c>
-      <c r="AR14" s="2">
+      <c r="AR14" s="4">
         <v>1.6803088803088808</v>
       </c>
-      <c r="AS14" s="2">
+      <c r="AS14" s="4">
         <v>1.75938223938224</v>
       </c>
-      <c r="AT14" s="2">
+      <c r="AT14" s="4">
         <v>1.8582239382239385</v>
       </c>
-      <c r="AU14" s="2">
+      <c r="AU14" s="4">
         <v>1.9372972972972982</v>
       </c>
-      <c r="AV14" s="2">
+      <c r="AV14" s="4">
         <v>1.9768339768339773</v>
       </c>
-      <c r="AW14" s="2">
+      <c r="AW14" s="4">
         <v>1.7791505791505797</v>
       </c>
-      <c r="AX14" s="2">
+      <c r="AX14" s="4">
         <v>1.7198455598455602</v>
       </c>
-      <c r="AY14" s="2">
+      <c r="AY14" s="4">
         <v>1.6210038610038611</v>
       </c>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="4">
         <v>13.5</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="4">
         <v>11.008494208494213</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="4">
         <v>9.6741312741312768</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="4">
         <v>8.6733590733590766</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="4">
         <v>8.3397683397683426</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="4">
         <v>10.007722007722011</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="4">
         <v>11.675675675675679</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="4">
         <v>13.010038610038615</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="4">
         <v>13.677220077220079</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="4">
         <v>14.677992277992283</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L15" s="4">
         <v>14.844787644787649</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M15" s="4">
         <v>14.010810810810815</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N15" s="4">
         <v>13.343629343629347</v>
       </c>
-      <c r="O15" s="2">
+      <c r="O15" s="4">
         <v>12.676447876447879</v>
       </c>
-      <c r="P15" s="2">
+      <c r="P15" s="4">
         <v>14.677992277992283</v>
       </c>
-      <c r="Q15" s="2">
+      <c r="Q15" s="4">
         <v>15.011583011583015</v>
       </c>
-      <c r="R15" s="2">
+      <c r="R15" s="4">
         <v>14.177606177606181</v>
       </c>
-      <c r="S15" s="2">
+      <c r="S15" s="4">
         <v>14.844787644787649</v>
       </c>
-      <c r="T15" s="2">
+      <c r="T15" s="4">
         <v>15.67876447876448</v>
       </c>
-      <c r="U15" s="2">
+      <c r="U15" s="4">
         <v>16.345945945945953</v>
       </c>
-      <c r="V15" s="2">
+      <c r="V15" s="4">
         <v>16.679536679536685</v>
       </c>
-      <c r="W15" s="2">
+      <c r="W15" s="4">
         <v>15.011583011583015</v>
       </c>
-      <c r="X15" s="2">
+      <c r="X15" s="4">
         <v>14.511196911196913</v>
       </c>
-      <c r="Y15" s="2">
+      <c r="Y15" s="4">
         <v>13.677220077220079</v>
       </c>
       <c r="AA15" t="s">
         <v>31</v>
       </c>
-      <c r="AB15" s="2">
+      <c r="AB15" s="4">
         <v>5.8</v>
       </c>
-      <c r="AC15" s="2">
+      <c r="AC15" s="4">
         <v>4.7295752895752914</v>
       </c>
-      <c r="AD15" s="2">
+      <c r="AD15" s="4">
         <v>4.1562934362934376</v>
       </c>
-      <c r="AE15" s="2">
+      <c r="AE15" s="4">
         <v>3.7263320463320473</v>
       </c>
-      <c r="AF15" s="2">
+      <c r="AF15" s="4">
         <v>3.5830115830115838</v>
       </c>
-      <c r="AG15" s="2">
+      <c r="AG15" s="4">
         <v>4.2996138996139006</v>
       </c>
-      <c r="AH15" s="2">
+      <c r="AH15" s="4">
         <v>5.0162162162162174</v>
       </c>
-      <c r="AI15" s="2">
+      <c r="AI15" s="4">
         <v>5.5894980694980712</v>
       </c>
-      <c r="AJ15" s="2">
+      <c r="AJ15" s="4">
         <v>5.8761389961389972</v>
       </c>
-      <c r="AK15" s="2">
+      <c r="AK15" s="4">
         <v>6.3061003861003879</v>
       </c>
-      <c r="AL15" s="2">
+      <c r="AL15" s="4">
         <v>6.377760617760619</v>
       </c>
-      <c r="AM15" s="2">
+      <c r="AM15" s="4">
         <v>6.019459459459461</v>
       </c>
-      <c r="AN15" s="2">
+      <c r="AN15" s="4">
         <v>5.7328185328185342</v>
       </c>
-      <c r="AO15" s="2">
+      <c r="AO15" s="4">
         <v>5.4461776061776073</v>
       </c>
-      <c r="AP15" s="2">
+      <c r="AP15" s="4">
         <v>6.3061003861003879</v>
       </c>
-      <c r="AQ15" s="2">
+      <c r="AQ15" s="4">
         <v>6.4494208494208509</v>
       </c>
-      <c r="AR15" s="2">
+      <c r="AR15" s="4">
         <v>6.091119691119693</v>
       </c>
-      <c r="AS15" s="2">
+      <c r="AS15" s="4">
         <v>6.377760617760619</v>
       </c>
-      <c r="AT15" s="2">
+      <c r="AT15" s="4">
         <v>6.736061776061776</v>
       </c>
-      <c r="AU15" s="2">
+      <c r="AU15" s="4">
         <v>7.0227027027027056</v>
       </c>
-      <c r="AV15" s="2">
+      <c r="AV15" s="4">
         <v>7.1660231660231677</v>
       </c>
-      <c r="AW15" s="2">
+      <c r="AW15" s="4">
         <v>6.4494208494208509</v>
       </c>
-      <c r="AX15" s="2">
+      <c r="AX15" s="4">
         <v>6.2344401544401551</v>
       </c>
-      <c r="AY15" s="2">
+      <c r="AY15" s="4">
         <v>5.8761389961389972</v>
       </c>
     </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="4">
         <v>14.9</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="4">
         <v>12.150115830115833</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="4">
         <v>10.67737451737452</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="4">
         <v>9.5728185328185358</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="4">
         <v>9.2046332046332076</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="4">
         <v>11.045559845559849</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="4">
         <v>12.88648648648649</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="4">
         <v>14.359227799227805</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="4">
         <v>15.095598455598457</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="4">
         <v>16.200154440154446</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16" s="4">
         <v>16.384247104247109</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M16" s="4">
         <v>15.463783783783787</v>
       </c>
-      <c r="N16" s="2">
+      <c r="N16" s="4">
         <v>14.727413127413131</v>
       </c>
-      <c r="O16" s="2">
+      <c r="O16" s="4">
         <v>13.991042471042475</v>
       </c>
-      <c r="P16" s="2">
+      <c r="P16" s="4">
         <v>16.200154440154446</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="Q16" s="4">
         <v>16.568339768339772</v>
       </c>
-      <c r="R16" s="2">
+      <c r="R16" s="4">
         <v>15.647876447876452</v>
       </c>
-      <c r="S16" s="2">
+      <c r="S16" s="4">
         <v>16.384247104247109</v>
       </c>
-      <c r="T16" s="2">
+      <c r="T16" s="4">
         <v>17.304710424710425</v>
       </c>
-      <c r="U16" s="2">
+      <c r="U16" s="4">
         <v>18.041081081081085</v>
       </c>
-      <c r="V16" s="2">
+      <c r="V16" s="4">
         <v>18.409266409266415</v>
       </c>
-      <c r="W16" s="2">
+      <c r="W16" s="4">
         <v>16.568339768339772</v>
       </c>
-      <c r="X16" s="2">
+      <c r="X16" s="4">
         <v>16.016061776061779</v>
       </c>
-      <c r="Y16" s="2">
+      <c r="Y16" s="4">
         <v>15.095598455598457</v>
       </c>
       <c r="AA16" t="s">
         <v>32</v>
       </c>
-      <c r="AB16" s="2">
+      <c r="AB16" s="4">
         <v>5</v>
       </c>
-      <c r="AC16" s="2">
+      <c r="AC16" s="4">
         <v>4.0772200772200788</v>
       </c>
-      <c r="AD16" s="2">
+      <c r="AD16" s="4">
         <v>3.5830115830115838</v>
       </c>
-      <c r="AE16" s="2">
+      <c r="AE16" s="4">
         <v>3.2123552123552135</v>
       </c>
-      <c r="AF16" s="2">
+      <c r="AF16" s="4">
         <v>3.0888030888030897</v>
       </c>
-      <c r="AG16" s="2">
+      <c r="AG16" s="4">
         <v>3.7065637065637076</v>
       </c>
-      <c r="AH16" s="2">
+      <c r="AH16" s="4">
         <v>4.3243243243243255</v>
       </c>
-      <c r="AI16" s="2">
+      <c r="AI16" s="4">
         <v>4.8185328185328204</v>
       </c>
-      <c r="AJ16" s="2">
+      <c r="AJ16" s="4">
         <v>5.0656370656370662</v>
       </c>
-      <c r="AK16" s="2">
+      <c r="AK16" s="4">
         <v>5.4362934362934379</v>
       </c>
-      <c r="AL16" s="2">
+      <c r="AL16" s="4">
         <v>5.4980694980694995</v>
       </c>
-      <c r="AM16" s="2">
+      <c r="AM16" s="4">
         <v>5.1891891891891904</v>
       </c>
-      <c r="AN16" s="2">
+      <c r="AN16" s="4">
         <v>4.9420849420849438</v>
       </c>
-      <c r="AO16" s="2">
+      <c r="AO16" s="4">
         <v>4.6949806949806954</v>
       </c>
-      <c r="AP16" s="2">
+      <c r="AP16" s="4">
         <v>5.4362934362934379</v>
       </c>
-      <c r="AQ16" s="2">
+      <c r="AQ16" s="4">
         <v>5.5598455598455612</v>
       </c>
-      <c r="AR16" s="2">
+      <c r="AR16" s="4">
         <v>5.2509652509652529</v>
       </c>
-      <c r="AS16" s="2">
+      <c r="AS16" s="4">
         <v>5.4980694980694995</v>
       </c>
-      <c r="AT16" s="2">
+      <c r="AT16" s="4">
         <v>5.8069498069498069</v>
       </c>
-      <c r="AU16" s="2">
+      <c r="AU16" s="4">
         <v>6.0540540540540553</v>
       </c>
-      <c r="AV16" s="2">
+      <c r="AV16" s="4">
         <v>6.1776061776061795</v>
       </c>
-      <c r="AW16" s="2">
+      <c r="AW16" s="4">
         <v>5.5598455598455612</v>
       </c>
-      <c r="AX16" s="2">
+      <c r="AX16" s="4">
         <v>5.3745173745173753</v>
       </c>
-      <c r="AY16" s="2">
+      <c r="AY16" s="4">
         <v>5.0656370656370662</v>
       </c>
     </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -4326,7 +4286,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -4534,39 +4494,39 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.81640625" customWidth="1"/>
-    <col min="8" max="8" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4600,7 +4560,7 @@
       <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="5" t="s">
         <v>58</v>
       </c>
       <c r="M1" t="s">
@@ -4628,7 +4588,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -4668,7 +4628,7 @@
         <f>IF(L2&gt;0,MAX(I2,J2),-MAX(I2,J2))</f>
         <v>-8</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="5">
         <v>0</v>
       </c>
       <c r="M2">
@@ -4685,20 +4645,20 @@
       <c r="P2" t="s">
         <v>34</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="Q2" s="2">
         <v>0.4</v>
       </c>
-      <c r="R2" s="3">
+      <c r="R2" s="2">
         <v>0.7</v>
       </c>
-      <c r="S2" s="3">
+      <c r="S2" s="2">
         <v>0.2</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -4708,7 +4668,7 @@
       <c r="C3">
         <v>75</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3">
         <f t="shared" ref="D3:D8" si="0">C3*Q3</f>
         <v>7.5</v>
       </c>
@@ -4738,7 +4698,7 @@
         <f t="shared" ref="K3:K4" si="5">IF(L3&gt;0,MAX(I3,J3),-MAX(I3,J3))</f>
         <v>-4</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="5">
         <v>0</v>
       </c>
       <c r="M3">
@@ -4755,20 +4715,20 @@
       <c r="P3" t="s">
         <v>36</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="Q3" s="2">
         <v>0.1</v>
       </c>
-      <c r="R3" s="3">
+      <c r="R3" s="2">
         <v>0.7</v>
       </c>
-      <c r="S3" s="3">
+      <c r="S3" s="2">
         <v>0.3</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -4808,7 +4768,7 @@
         <f t="shared" si="5"/>
         <v>-4</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="5">
         <v>0</v>
       </c>
       <c r="M4">
@@ -4825,20 +4785,20 @@
       <c r="P4" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="Q4" s="2">
         <v>0.1</v>
       </c>
-      <c r="R4" s="3">
+      <c r="R4" s="2">
         <v>0.7</v>
       </c>
-      <c r="S4" s="3">
+      <c r="S4" s="2">
         <v>0.3</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -4878,7 +4838,7 @@
         <f t="shared" ref="K5:K8" si="8">IF(L5&gt;0,MAX(I5,J5),-MAX(I5,J5))</f>
         <v>-4</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="5">
         <v>0</v>
       </c>
       <c r="M5">
@@ -4895,20 +4855,20 @@
       <c r="P5" t="s">
         <v>36</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="Q5" s="2">
         <v>0.1</v>
       </c>
-      <c r="R5" s="3">
+      <c r="R5" s="2">
         <v>0.7</v>
       </c>
-      <c r="S5" s="3">
+      <c r="S5" s="2">
         <v>0.3</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -4948,7 +4908,7 @@
         <f t="shared" si="8"/>
         <v>-4</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="5">
         <v>0</v>
       </c>
       <c r="M6">
@@ -4965,20 +4925,20 @@
       <c r="P6" t="s">
         <v>36</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="Q6" s="2">
         <v>0.1</v>
       </c>
-      <c r="R6" s="3">
+      <c r="R6" s="2">
         <v>0.7</v>
       </c>
-      <c r="S6" s="3">
+      <c r="S6" s="2">
         <v>0.3</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -4993,11 +4953,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="6">
         <f t="shared" si="1"/>
         <v>24.015179563180958</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="6">
         <f t="shared" si="2"/>
         <v>-24.015179563180958</v>
       </c>
@@ -5019,7 +4979,7 @@
         <f t="shared" si="8"/>
         <v>-1</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="5">
         <v>0</v>
       </c>
       <c r="M7">
@@ -5036,20 +4996,20 @@
       <c r="P7" t="s">
         <v>79</v>
       </c>
-      <c r="Q7" s="1">
-        <v>0</v>
-      </c>
-      <c r="R7" s="3">
+      <c r="Q7" s="2">
+        <v>0</v>
+      </c>
+      <c r="R7" s="2">
         <v>0.7</v>
       </c>
-      <c r="S7" s="3">
+      <c r="S7" s="2">
         <v>10</v>
       </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>76</v>
       </c>
@@ -5064,11 +5024,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="6">
         <f t="shared" si="1"/>
         <v>25.264257373812136</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="6">
         <f t="shared" si="2"/>
         <v>-25.264257373812136</v>
       </c>
@@ -5090,7 +5050,7 @@
         <f t="shared" si="8"/>
         <v>-1</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="5">
         <v>0</v>
       </c>
       <c r="M8">
@@ -5107,22 +5067,27 @@
       <c r="P8" t="s">
         <v>80</v>
       </c>
-      <c r="Q8" s="1">
-        <v>0</v>
-      </c>
-      <c r="R8" s="3">
+      <c r="Q8" s="2">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2">
         <v>0.7</v>
       </c>
-      <c r="S8" s="3">
+      <c r="S8" s="2">
         <v>10</v>
       </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -5131,26 +5096,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -5173,7 +5136,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -5196,7 +5159,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -5219,7 +5182,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -5242,7 +5205,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -5265,7 +5228,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -5288,7 +5251,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -5311,7 +5274,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -5334,7 +5297,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -5357,7 +5320,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -5380,7 +5343,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -5403,7 +5366,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -5426,7 +5389,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -5449,7 +5412,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -5472,7 +5435,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -5495,7 +5458,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -5518,7 +5481,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -5541,7 +5504,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -5564,7 +5527,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -5587,7 +5550,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -5610,7 +5573,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -5633,7 +5596,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -5645,25 +5608,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>81</v>
       </c>
@@ -5740,166 +5701,166 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="4">
         <v>31.167028084846212</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="4">
         <v>29.425609562813513</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <v>27.672290686345676</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="4">
         <v>28.632252604835134</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="4">
         <v>28.751256148226485</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="4">
         <v>29.223303538341348</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="4">
         <v>28.636219389714864</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="4">
         <v>29.738985560973511</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="4">
         <v>30.42127254455378</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="4">
         <v>31.766012587993242</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="4">
         <v>33.130586555397841</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="4">
         <v>36.407150790836482</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="4">
         <v>38.46194531159189</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3" s="4">
         <v>40.528640186164324</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="4">
         <v>41.393399270022165</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3" s="4">
         <v>42.515999365423781</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R3" s="4">
         <v>45.495054741662159</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3" s="4">
         <v>42.611202200418106</v>
       </c>
-      <c r="T3" s="2">
+      <c r="T3" s="4">
         <v>37.747924049807295</v>
       </c>
-      <c r="U3" s="2">
+      <c r="U3" s="4">
         <v>34.487226953035673</v>
       </c>
-      <c r="V3" s="2">
+      <c r="V3" s="4">
         <v>35.982704818522699</v>
       </c>
-      <c r="W3" s="2">
+      <c r="W3" s="4">
         <v>35.470989580551617</v>
       </c>
-      <c r="X3" s="2">
+      <c r="X3" s="4">
         <v>32.503834558452162</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="Y3" s="4">
         <v>31.206695932817297</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
         <v>1.4809329877823026E-4</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="4">
         <v>7.1452054794520539</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="4">
         <v>32.11573491299513</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="4">
         <v>64.624361347648914</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="4">
         <v>84.546612365790267</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="4">
         <v>90.860273972602698</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="4">
         <v>92.644353942984054</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="4">
         <v>93.031099592743232</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="4">
         <v>92.748019252128643</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="4">
         <v>91.194002221399458</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="4">
         <v>86.714328026656744</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q4" s="4">
         <v>73.326471677156476</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4" s="4">
         <v>41.897519437245407</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4" s="4">
         <v>14.732839689004052</v>
       </c>
-      <c r="T4" s="2">
+      <c r="T4" s="4">
         <v>0.62213994816734319</v>
       </c>
-      <c r="U4" s="2">
-        <v>0</v>
-      </c>
-      <c r="V4" s="2">
-        <v>0</v>
-      </c>
-      <c r="W4" s="2">
-        <v>0</v>
-      </c>
-      <c r="X4" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="U4" s="4">
+        <v>0</v>
+      </c>
+      <c r="V4" s="4">
+        <v>0</v>
+      </c>
+      <c r="W4" s="4">
+        <v>0</v>
+      </c>
+      <c r="X4" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -6000,7 +5961,7 @@
         <v>262.40000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>82</v>
       </c>
@@ -6101,7 +6062,7 @@
         <v>31.206695932817297</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -6202,7 +6163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>85</v>
       </c>
@@ -6303,29 +6264,29 @@
         <v>231.19330406718274</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>86</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="7">
         <f>AVERAGE(B8:Y8)/AVERAGE(B7:Y7)</f>
         <v>0.13422737847206598</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>87</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="7">
         <f>AVERAGE(B9:Y9)/AVERAGE(B7:Y7)</f>
         <v>0.14120881450870093</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>88</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="7">
         <f>D28+D29</f>
         <v>0.27543619298076694</v>
       </c>

</xml_diff>